<commit_message>
Quality control on fibrosis chip and subsequent Mmp10 removal
</commit_message>
<xml_diff>
--- a/BDLanalysis/inst/extdata/raw_data.xlsx
+++ b/BDLanalysis/inst/extdata/raw_data.xlsx
@@ -306,13 +306,13 @@
     <t>ALT</t>
   </si>
   <si>
-    <t>sid_Bilirubin</t>
-  </si>
-  <si>
-    <t>pid_Bilirubin</t>
-  </si>
-  <si>
-    <t>Bilirubin</t>
+    <t>sid_bilirubin</t>
+  </si>
+  <si>
+    <t>pid_bilirubin</t>
+  </si>
+  <si>
+    <t>bilirubin</t>
   </si>
   <si>
     <t>sid_albumin</t>
@@ -351,13 +351,13 @@
     <t>BrdU_Kupffer</t>
   </si>
   <si>
-    <t>sid_BrdU_HSC</t>
-  </si>
-  <si>
-    <t>pid_BrdU_HSC</t>
-  </si>
-  <si>
-    <t>BrdU_HSC</t>
+    <t>sid_BrdU_BEC</t>
+  </si>
+  <si>
+    <t>pid_BrdU_BEC</t>
+  </si>
+  <si>
+    <t>BrdU_BEC</t>
   </si>
   <si>
     <t>sid_BrdU_SiriusRed</t>
@@ -1411,7 +1411,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1584,10 +1584,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1708,7 +1704,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2570,8 +2566,8 @@
   </sheetPr>
   <dimension ref="A1:AE42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE45" activeCellId="0" sqref="AE45"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -6491,7 +6487,7 @@
   <dimension ref="1:42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AW2" activeCellId="0" sqref="AW2"/>
+      <selection pane="topLeft" activeCell="AW2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -13818,7 +13814,7 @@
   <dimension ref="1:42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AW2" activeCellId="0" sqref="AW2"/>
+      <selection pane="topLeft" activeCell="AW2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -21086,7 +21082,7 @@
   <dimension ref="A1:AX42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -27380,7 +27376,7 @@
   <dimension ref="1:42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AW42" activeCellId="0" sqref="AW42"/>
+      <selection pane="topLeft" activeCell="AW42" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -34693,10 +34689,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -34875,7 +34871,6 @@
       <c r="E10" s="0" t="s">
         <v>414</v>
       </c>
-      <c r="F10" s="43"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="41" t="n">
@@ -34898,7 +34893,7 @@
       <c r="A12" s="41" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="43" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="42" t="n">
@@ -34915,7 +34910,7 @@
       <c r="A13" s="41" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="43" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="42" t="n">
@@ -35148,7 +35143,6 @@
       <c r="E26" s="0" t="s">
         <v>414</v>
       </c>
-      <c r="F26" s="43"/>
     </row>
     <row r="27" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="41" t="n">
@@ -35217,7 +35211,6 @@
       <c r="E30" s="0" t="s">
         <v>414</v>
       </c>
-      <c r="F30" s="43"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="41" t="n">
@@ -35235,7 +35228,6 @@
       <c r="E31" s="0" t="s">
         <v>414</v>
       </c>
-      <c r="F31" s="43"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="41" t="n">
@@ -35389,7 +35381,6 @@
       <c r="E40" s="0" t="s">
         <v>414</v>
       </c>
-      <c r="F40" s="43"/>
     </row>
     <row r="41" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="41" t="n">
@@ -35427,14 +35418,14 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J33" activeCellId="0" sqref="J33"/>
+      <selection pane="topLeft" activeCell="J33" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="45" width="14.7244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="45" width="16.8112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="45" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="44" width="14.7244897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="16.8112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="44" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35486,11 +35477,11 @@
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="41" t="n">
@@ -35499,11 +35490,11 @@
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="41" t="n">
@@ -35512,11 +35503,11 @@
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="41" t="n">
@@ -35525,11 +35516,11 @@
       <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="41" t="n">
@@ -35538,11 +35529,11 @@
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="41" t="n">
@@ -35551,11 +35542,11 @@
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="41" t="n">
@@ -35564,11 +35555,11 @@
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="41" t="n">
@@ -35577,11 +35568,11 @@
       <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="41" t="n">
@@ -35590,11 +35581,11 @@
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="41" t="n">
@@ -35603,11 +35594,11 @@
       <c r="B12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="n">
@@ -35616,11 +35607,11 @@
       <c r="B13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="41" t="n">
@@ -35629,11 +35620,11 @@
       <c r="B14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="41" t="n">
@@ -35642,11 +35633,11 @@
       <c r="B15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="41" t="n">
@@ -35655,11 +35646,11 @@
       <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="41" t="n">
@@ -35668,11 +35659,11 @@
       <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="41" t="n">
@@ -35681,11 +35672,11 @@
       <c r="B18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="41" t="n">
@@ -35694,11 +35685,11 @@
       <c r="B19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="41" t="n">
@@ -35707,11 +35698,11 @@
       <c r="B20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="41" t="n">
@@ -35720,11 +35711,11 @@
       <c r="B21" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="41" t="n">
@@ -35733,11 +35724,11 @@
       <c r="B22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="41" t="n">
@@ -35746,11 +35737,11 @@
       <c r="B23" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="41" t="n">
@@ -35759,11 +35750,11 @@
       <c r="B24" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="41" t="n">
@@ -35772,11 +35763,11 @@
       <c r="B25" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="46"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="41" t="n">
@@ -35785,11 +35776,11 @@
       <c r="B26" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="41" t="n">
@@ -35798,11 +35789,11 @@
       <c r="B27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="46"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="41" t="n">
@@ -35811,11 +35802,11 @@
       <c r="B28" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="46"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="41" t="n">
@@ -35824,11 +35815,11 @@
       <c r="B29" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="41" t="n">
@@ -35837,11 +35828,11 @@
       <c r="B30" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="41" t="n">
@@ -35850,11 +35841,11 @@
       <c r="B31" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="41" t="n">
@@ -35863,11 +35854,11 @@
       <c r="B32" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="46"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="41" t="n">
@@ -35876,11 +35867,11 @@
       <c r="B33" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="46"/>
-      <c r="D33" s="46"/>
-      <c r="E33" s="46"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="46"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="41" t="n">
@@ -35889,11 +35880,11 @@
       <c r="B34" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="41" t="n">
@@ -35902,11 +35893,11 @@
       <c r="B35" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="46"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="46"/>
-      <c r="F35" s="46"/>
-      <c r="G35" s="46"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="41" t="n">
@@ -35915,11 +35906,11 @@
       <c r="B36" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C36" s="46"/>
-      <c r="D36" s="46"/>
-      <c r="E36" s="46"/>
-      <c r="F36" s="46"/>
-      <c r="G36" s="46"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="41" t="n">
@@ -35928,11 +35919,11 @@
       <c r="B37" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C37" s="46"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="46"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="45"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="41" t="n">
@@ -35941,11 +35932,11 @@
       <c r="B38" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C38" s="46"/>
-      <c r="D38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="46"/>
-      <c r="G38" s="46"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="45"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="41" t="n">
@@ -35954,11 +35945,11 @@
       <c r="B39" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="46"/>
-      <c r="D39" s="46"/>
-      <c r="E39" s="46"/>
-      <c r="F39" s="46"/>
-      <c r="G39" s="46"/>
+      <c r="C39" s="45"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="45"/>
+      <c r="G39" s="45"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="41" t="n">
@@ -35967,11 +35958,11 @@
       <c r="B40" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="46"/>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="46"/>
-      <c r="G40" s="46"/>
+      <c r="C40" s="45"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="45"/>
+      <c r="G40" s="45"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="41" t="n">
@@ -35980,11 +35971,11 @@
       <c r="B41" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C41" s="46"/>
-      <c r="D41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="46"/>
-      <c r="G41" s="46"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="45"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="41" t="n">
@@ -35993,11 +35984,11 @@
       <c r="B42" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C42" s="46"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="46"/>
+      <c r="C42" s="45"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="45"/>
+      <c r="G42" s="45"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Update of factor names and last manuscript version
</commit_message>
<xml_diff>
--- a/BDLanalysis/inst/extdata/raw_data.xlsx
+++ b/BDLanalysis/inst/extdata/raw_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="536" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="536" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="samples" sheetId="1" state="visible" r:id="rId2"/>
@@ -1263,7 +1263,7 @@
     <t>CTGF</t>
   </si>
   <si>
-    <t>S100A4</t>
+    <t>S100a4</t>
   </si>
   <si>
     <t>NA</t>
@@ -1704,7 +1704,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2566,8 +2566,8 @@
   </sheetPr>
   <dimension ref="A1:AE42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -6487,7 +6487,7 @@
   <dimension ref="1:42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AW2" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="AW2" activeCellId="0" sqref="AW2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -13814,7 +13814,7 @@
   <dimension ref="1:42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AW2" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="AW2" activeCellId="0" sqref="AW2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -21082,7 +21082,7 @@
   <dimension ref="A1:AX42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -27376,7 +27376,7 @@
   <dimension ref="1:42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AW42" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="AW42" activeCellId="0" sqref="AW42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -34691,8 +34691,8 @@
   </sheetPr>
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -35418,7 +35418,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J33" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="J33" activeCellId="0" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>